<commit_message>
prepare project; prepare data; descriptives for RQ1
</commit_message>
<xml_diff>
--- a/_data/zuordnung_new_task.xlsx
+++ b/_data/zuordnung_new_task.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boehm\Documents\01_Work\01_Uni-MA\01_Forschung\02_AARL-BS\06_Veröffentlichungen\Vocational Teachers' Informal WPL\_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boehm\Documents\01_Work\01_Uni-MA\01_Forschung\02_AARL-BS\06_Veröffentlichungen\Karasek_Special-Issue\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAFAD2E-8B2E-4C61-8E3A-9135D23890DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D5A9D6-16A2-4C1D-BF10-5507B0064176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CA4B50BC-CD78-4C0C-9EB5-40D7F8343EC1}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="zuordnung_new_task" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">zuordnung_new_task!$A$1:$G$30</definedName>
+    <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">zuordnung_new_task!$A$1:$H$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="90">
   <si>
     <t>alte_kategorie</t>
   </si>
@@ -284,6 +284,39 @@
   </si>
   <si>
     <t>Recurring service routes</t>
+  </si>
+  <si>
+    <t>taskname_new_en</t>
+  </si>
+  <si>
+    <t>Preparation and follow-up of lessons</t>
+  </si>
+  <si>
+    <t>Organizational tasks</t>
+  </si>
+  <si>
+    <t>Non-formal training</t>
+  </si>
+  <si>
+    <t>Formal training</t>
+  </si>
+  <si>
+    <t>Personnel management</t>
+  </si>
+  <si>
+    <t>Official interaction with external parties and administrative bodies</t>
+  </si>
+  <si>
+    <t>Leadership of committees and teams</t>
+  </si>
+  <si>
+    <t>Participation in committees and teams</t>
+  </si>
+  <si>
+    <t>Official interaction with colleagues</t>
+  </si>
+  <si>
+    <t>Interaction with students outside the classroom</t>
   </si>
 </sst>
 </file>
@@ -319,9 +352,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -354,13 +386,14 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExterneDaten_1" connectionId="1" xr16:uid="{04F32AC9-34AF-44B8-95C4-5B62EAB8C631}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="8">
-    <queryTableFields count="7">
+  <queryTableRefresh nextId="9">
+    <queryTableFields count="8">
       <queryTableField id="1" name="alte_kategorie" tableColumnId="1"/>
       <queryTableField id="2" name="task_name" tableColumnId="2"/>
       <queryTableField id="7" dataBound="0" tableColumnId="7"/>
       <queryTableField id="3" name="neue_kategorie" tableColumnId="3"/>
       <queryTableField id="4" name="taskname_new" tableColumnId="4"/>
+      <queryTableField id="8" dataBound="0" tableColumnId="8"/>
       <queryTableField id="5" name="category_three" tableColumnId="5"/>
       <queryTableField id="6" name="taskname_three" tableColumnId="6"/>
     </queryTableFields>
@@ -369,16 +402,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DE54EC4-36DF-4ADA-90C4-EF4B8B9F92CC}" name="zuordnung_new_task" displayName="zuordnung_new_task" ref="A1:G30" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:G30" xr:uid="{3DE54EC4-36DF-4ADA-90C4-EF4B8B9F92CC}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DE54EC4-36DF-4ADA-90C4-EF4B8B9F92CC}" name="zuordnung_new_task" displayName="zuordnung_new_task" ref="A1:H30" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:H30" xr:uid="{3DE54EC4-36DF-4ADA-90C4-EF4B8B9F92CC}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{A9C04F7D-398B-40D9-A4CE-4259A167D6C2}" uniqueName="1" name="alte_kategorie" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{38F8BFC6-D86D-4066-B2A6-6831860BB9A9}" uniqueName="2" name="task_name" queryTableFieldId="2" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{6873F729-DF2E-428F-8112-74A8C2215478}" uniqueName="7" name="task_name_en" queryTableFieldId="7" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{6873F729-DF2E-428F-8112-74A8C2215478}" uniqueName="7" name="task_name_en" queryTableFieldId="7" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{85CEBFB8-3FAF-477A-9A2E-39CEC25A2CB6}" uniqueName="3" name="neue_kategorie" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{C3C655D1-D675-47F3-8CDC-17CF66F9B758}" uniqueName="4" name="taskname_new" queryTableFieldId="4" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{C3C655D1-D675-47F3-8CDC-17CF66F9B758}" uniqueName="4" name="taskname_new" queryTableFieldId="4" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{67BD0033-D4BC-41F4-AB10-B0449E8088D5}" uniqueName="8" name="taskname_new_en" queryTableFieldId="8"/>
     <tableColumn id="5" xr3:uid="{0B97A6D7-EE58-4834-94EF-A424D28BBD4D}" uniqueName="5" name="category_three" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{403255CF-896C-4B31-A117-0D614FA64567}" uniqueName="6" name="taskname_three" queryTableFieldId="6" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{403255CF-896C-4B31-A117-0D614FA64567}" uniqueName="6" name="taskname_three" queryTableFieldId="6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -701,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A86ADC4-DE4A-4DE5-9708-ACA49157EFD9}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,11 +748,12 @@
     <col min="3" max="3" width="55.5703125" customWidth="1"/>
     <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="51.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -735,670 +770,763 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>51</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2">
         <v>1</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>77</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>76</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G4">
         <v>2</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>66</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>52</v>
       </c>
       <c r="D6">
         <v>3</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>53</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>19</v>
       </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>54</v>
       </c>
       <c r="D8">
         <v>11</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>21</v>
       </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>55</v>
       </c>
       <c r="D9">
         <v>4</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>14</v>
       </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>56</v>
       </c>
       <c r="D10">
         <v>4</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>14</v>
       </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="D11">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>78</v>
       </c>
       <c r="D12">
         <v>12</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>27</v>
       </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>58</v>
       </c>
       <c r="D13">
         <v>6</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>29</v>
       </c>
-      <c r="F13">
-        <v>3</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>59</v>
       </c>
       <c r="D14">
         <v>7</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>31</v>
       </c>
-      <c r="F14">
-        <v>3</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>60</v>
       </c>
       <c r="D15">
         <v>12</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>27</v>
       </c>
-      <c r="F15">
-        <v>3</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="H15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>61</v>
       </c>
       <c r="D16">
         <v>4</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>14</v>
       </c>
-      <c r="F16">
-        <v>3</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>62</v>
       </c>
       <c r="D17">
         <v>8</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>35</v>
       </c>
-      <c r="F17">
-        <v>3</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>87</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>63</v>
       </c>
       <c r="D18">
         <v>8</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>35</v>
       </c>
-      <c r="F18">
-        <v>3</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>64</v>
       </c>
       <c r="D19">
         <v>8</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>35</v>
       </c>
-      <c r="F19">
-        <v>3</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>87</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>65</v>
       </c>
       <c r="D20">
         <v>12</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>27</v>
       </c>
-      <c r="F20">
-        <v>3</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>67</v>
       </c>
       <c r="D21">
         <v>12</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>27</v>
       </c>
-      <c r="F21">
-        <v>3</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>68</v>
       </c>
       <c r="D22">
         <v>8</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>35</v>
       </c>
-      <c r="F22">
-        <v>3</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>87</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>69</v>
       </c>
       <c r="D23">
         <v>9</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>42</v>
       </c>
-      <c r="F23">
-        <v>3</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
+      <c r="H23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>70</v>
       </c>
       <c r="D24">
         <v>9</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>42</v>
       </c>
-      <c r="F24">
-        <v>3</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>71</v>
       </c>
       <c r="D25">
         <v>4</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>14</v>
       </c>
-      <c r="F25">
-        <v>3</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>81</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+      <c r="H25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>72</v>
       </c>
       <c r="D26">
         <v>10</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>46</v>
       </c>
-      <c r="F26">
-        <v>3</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26">
+        <v>3</v>
+      </c>
+      <c r="H26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>73</v>
       </c>
       <c r="D27">
         <v>11</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>21</v>
       </c>
-      <c r="F27">
-        <v>3</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27">
+        <v>3</v>
+      </c>
+      <c r="H27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>74</v>
       </c>
       <c r="D28">
         <v>11</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>21</v>
       </c>
-      <c r="F28">
-        <v>3</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28">
+        <v>3</v>
+      </c>
+      <c r="H28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>54</v>
       </c>
       <c r="D29">
         <v>11</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>21</v>
       </c>
-      <c r="F29">
-        <v>3</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29">
+        <v>3</v>
+      </c>
+      <c r="H29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>75</v>
       </c>
       <c r="D30">
         <v>12</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>27</v>
       </c>
-      <c r="F30">
-        <v>3</v>
-      </c>
-      <c r="G30" s="1" t="s">
+      <c r="F30" t="s">
+        <v>75</v>
+      </c>
+      <c r="G30">
+        <v>3</v>
+      </c>
+      <c r="H30" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>